<commit_message>
This version produces good plot
</commit_message>
<xml_diff>
--- a/lab_report_2_time_series/modeling/Chris_versions/model_values_simple_11092014.xlsx
+++ b/lab_report_2_time_series/modeling/Chris_versions/model_values_simple_11092014.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="0" windowWidth="25600" windowHeight="14400"/>
+    <workbookView xWindow="5500" yWindow="0" windowWidth="25600" windowHeight="14400"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="90">
   <si>
     <t>x1</t>
   </si>
@@ -98,9 +98,6 @@
     <t>ERK</t>
   </si>
   <si>
-    <t>EGF to EGFR</t>
-  </si>
-  <si>
     <t>x11</t>
   </si>
   <si>
@@ -110,9 +107,6 @@
     <t>x13</t>
   </si>
   <si>
-    <t>EGF_EGFR dissociate</t>
-  </si>
-  <si>
     <t>actSOS</t>
   </si>
   <si>
@@ -128,9 +122,6 @@
     <t>actERK</t>
   </si>
   <si>
-    <t>SOS activation by EGF_EGFR</t>
-  </si>
-  <si>
     <t>SOS deactivation</t>
   </si>
   <si>
@@ -239,9 +230,6 @@
     <t>x18</t>
   </si>
   <si>
-    <t>TGFaAct</t>
-  </si>
-  <si>
     <t>x19</t>
   </si>
   <si>
@@ -257,7 +245,7 @@
     <t>actEGF_EGFR dissociate</t>
   </si>
   <si>
-    <t>act</t>
+    <t>actTGFa</t>
   </si>
   <si>
     <t>actTGFa_EGFR dissociate</t>
@@ -270,6 +258,39 @@
   </si>
   <si>
     <t>k20</t>
+  </si>
+  <si>
+    <t>actTGFa_EGFR</t>
+  </si>
+  <si>
+    <t>x20</t>
+  </si>
+  <si>
+    <t>SOS activation by actEGF_EGFR</t>
+  </si>
+  <si>
+    <t>k21</t>
+  </si>
+  <si>
+    <t>SOS activation by actEGFa_EGFR</t>
+  </si>
+  <si>
+    <t>actTACE cleaves EGF</t>
+  </si>
+  <si>
+    <t>actTACE cleaves TGFa</t>
+  </si>
+  <si>
+    <t>actTACE</t>
+  </si>
+  <si>
+    <t>TACE activation by actERK</t>
+  </si>
+  <si>
+    <t>k22</t>
+  </si>
+  <si>
+    <t>x21</t>
   </si>
 </sst>
 </file>
@@ -325,8 +346,50 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="123">
+  <cellStyleXfs count="165">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -458,7 +521,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="123">
+  <cellStyles count="165">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -520,6 +583,27 @@
     <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -581,6 +665,27 @@
     <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -880,79 +985,87 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC30"/>
+  <dimension ref="A1:AE30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="12.83203125" customWidth="1"/>
-    <col min="23" max="23" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.1640625" customWidth="1"/>
+    <col min="25" max="25" width="25.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:28">
       <c r="C1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D1" t="s">
         <v>19</v>
       </c>
       <c r="E1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F1" t="s">
         <v>20</v>
       </c>
       <c r="G1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H1" t="s">
         <v>21</v>
       </c>
       <c r="I1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J1" t="s">
         <v>22</v>
       </c>
       <c r="K1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L1" t="s">
         <v>23</v>
       </c>
       <c r="M1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="N1" t="s">
         <v>24</v>
       </c>
       <c r="O1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="P1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="Q1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="R1" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="S1" t="s">
         <v>18</v>
       </c>
       <c r="T1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="U1" t="s">
-        <v>72</v>
+        <v>74</v>
+      </c>
+      <c r="V1" t="s">
+        <v>79</v>
+      </c>
+      <c r="W1" t="s">
+        <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:28">
       <c r="C2" t="s">
         <v>0</v>
       </c>
@@ -984,42 +1097,48 @@
         <v>9</v>
       </c>
       <c r="M2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" t="s">
         <v>26</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>27</v>
       </c>
-      <c r="O2" t="s">
-        <v>28</v>
-      </c>
       <c r="P2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="Q2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="R2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="S2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="T2" t="s">
+        <v>68</v>
+      </c>
+      <c r="U2" t="s">
+        <v>69</v>
+      </c>
+      <c r="V2" t="s">
+        <v>80</v>
+      </c>
+      <c r="W2" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28">
+      <c r="A3" t="s">
         <v>71</v>
-      </c>
-      <c r="U2" t="s">
-        <v>73</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>17</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26">
-      <c r="A3" t="s">
-        <v>75</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -1081,22 +1200,28 @@
       <c r="U3">
         <v>0</v>
       </c>
-      <c r="W3" t="s">
-        <v>25</v>
-      </c>
-      <c r="X3" t="s">
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z3" t="s">
         <v>10</v>
       </c>
-      <c r="Y3">
+      <c r="AA3">
         <v>1E-3</v>
       </c>
-      <c r="Z3">
+      <c r="AB3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:28">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -1158,22 +1283,28 @@
       <c r="U4">
         <v>0</v>
       </c>
-      <c r="W4" t="s">
-        <v>29</v>
-      </c>
-      <c r="X4" t="s">
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z4" t="s">
         <v>11</v>
       </c>
-      <c r="Y4">
+      <c r="AA4">
         <v>0.01</v>
       </c>
-      <c r="Z4">
+      <c r="AB4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:28">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
@@ -1235,22 +1366,28 @@
       <c r="U5">
         <v>0</v>
       </c>
-      <c r="W5" t="s">
-        <v>35</v>
-      </c>
-      <c r="X5" t="s">
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z5" t="s">
         <v>12</v>
       </c>
-      <c r="Y5">
+      <c r="AA5">
         <v>1E-3</v>
       </c>
-      <c r="Z5">
+      <c r="AB5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:28">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
@@ -1312,22 +1449,28 @@
       <c r="U6">
         <v>0</v>
       </c>
-      <c r="W6" t="s">
-        <v>36</v>
-      </c>
-      <c r="X6" t="s">
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z6" t="s">
         <v>13</v>
       </c>
-      <c r="Y6">
+      <c r="AA6">
         <v>0.01</v>
       </c>
-      <c r="Z6">
+      <c r="AB6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:28">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
@@ -1389,22 +1532,28 @@
       <c r="U7">
         <v>0</v>
       </c>
-      <c r="W7" t="s">
-        <v>47</v>
-      </c>
-      <c r="X7" t="s">
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z7" t="s">
         <v>14</v>
       </c>
-      <c r="Y7">
+      <c r="AA7">
         <v>1E-3</v>
       </c>
-      <c r="Z7">
+      <c r="AB7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:28">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
@@ -1466,25 +1615,31 @@
       <c r="U8">
         <v>0</v>
       </c>
-      <c r="W8" t="s">
-        <v>37</v>
-      </c>
-      <c r="X8" t="s">
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z8" t="s">
         <v>15</v>
       </c>
-      <c r="Y8">
+      <c r="AA8">
         <v>0.01</v>
       </c>
-      <c r="Z8">
+      <c r="AB8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:28">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1543,25 +1698,31 @@
       <c r="U9">
         <v>0</v>
       </c>
-      <c r="W9" t="s">
-        <v>48</v>
-      </c>
-      <c r="X9" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y9">
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA9">
         <v>1E-3</v>
       </c>
-      <c r="Z9">
+      <c r="AB9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:28">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1620,25 +1781,31 @@
       <c r="U10">
         <v>0</v>
       </c>
-      <c r="W10" t="s">
-        <v>38</v>
-      </c>
-      <c r="X10" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y10">
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA10">
         <v>0.01</v>
       </c>
-      <c r="Z10">
+      <c r="AB10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:28">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1697,25 +1864,31 @@
       <c r="U11">
         <v>0</v>
       </c>
-      <c r="W11" t="s">
-        <v>49</v>
-      </c>
-      <c r="X11" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y11">
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA11">
         <v>1E-3</v>
       </c>
-      <c r="Z11">
+      <c r="AB11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:28">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1774,25 +1947,31 @@
       <c r="U12">
         <v>0</v>
       </c>
-      <c r="W12" t="s">
-        <v>39</v>
-      </c>
-      <c r="X12" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y12">
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA12">
         <v>0.01</v>
       </c>
-      <c r="Z12">
+      <c r="AB12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:28">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1851,25 +2030,31 @@
       <c r="U13">
         <v>0</v>
       </c>
-      <c r="W13" t="s">
-        <v>50</v>
-      </c>
-      <c r="X13" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y13">
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA13">
         <v>1E-3</v>
       </c>
-      <c r="Z13">
+      <c r="AB13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:28">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1928,25 +2113,31 @@
       <c r="U14">
         <v>0</v>
       </c>
-      <c r="W14" t="s">
-        <v>40</v>
-      </c>
-      <c r="X14" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y14">
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <v>0</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA14">
         <v>0.01</v>
       </c>
-      <c r="Z14">
+      <c r="AB14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:28">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1982,11 +2173,11 @@
         <v>0</v>
       </c>
       <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
         <v>-1</v>
       </c>
-      <c r="O15">
-        <v>0</v>
-      </c>
       <c r="P15">
         <v>1</v>
       </c>
@@ -2005,26 +2196,32 @@
       <c r="U15">
         <v>0</v>
       </c>
-      <c r="W15" t="s">
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>0</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA15">
+        <v>0.01</v>
+      </c>
+      <c r="AB15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28">
+      <c r="A16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" t="s">
         <v>51</v>
       </c>
-      <c r="X15" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y15">
-        <v>0.01</v>
-      </c>
-      <c r="Z15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26">
-      <c r="A16" t="s">
-        <v>58</v>
-      </c>
-      <c r="B16" t="s">
-        <v>54</v>
-      </c>
       <c r="C16">
         <v>0</v>
       </c>
@@ -2059,10 +2256,10 @@
         <v>0</v>
       </c>
       <c r="N16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P16">
         <v>-1</v>
@@ -2082,25 +2279,31 @@
       <c r="U16">
         <v>0</v>
       </c>
-      <c r="W16" t="s">
-        <v>58</v>
-      </c>
-      <c r="X16" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y16">
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>0</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA16">
         <v>1E-3</v>
       </c>
-      <c r="Z16">
+      <c r="AB16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:29">
+    <row r="17" spans="1:31">
       <c r="A17" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -2136,11 +2339,11 @@
         <v>0</v>
       </c>
       <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
         <v>-1</v>
       </c>
-      <c r="O17">
-        <v>0</v>
-      </c>
       <c r="P17">
         <v>0</v>
       </c>
@@ -2159,26 +2362,32 @@
       <c r="U17">
         <v>0</v>
       </c>
-      <c r="W17" t="s">
-        <v>52</v>
-      </c>
-      <c r="X17" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y17">
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA17">
         <v>0.01</v>
       </c>
-      <c r="Z17">
+      <c r="AB17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:29">
+    <row r="18" spans="1:31">
       <c r="A18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" t="s">
         <v>57</v>
       </c>
-      <c r="B18" t="s">
-        <v>60</v>
-      </c>
       <c r="C18">
         <v>0</v>
       </c>
@@ -2213,10 +2422,10 @@
         <v>0</v>
       </c>
       <c r="N18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P18">
         <v>0</v>
@@ -2236,25 +2445,31 @@
       <c r="U18">
         <v>0</v>
       </c>
-      <c r="W18" t="s">
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z18" t="s">
         <v>57</v>
       </c>
-      <c r="X18" t="s">
+      <c r="AA18">
+        <v>1E-3</v>
+      </c>
+      <c r="AB18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31">
+      <c r="A19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" t="s">
         <v>60</v>
-      </c>
-      <c r="Y18">
-        <v>1E-3</v>
-      </c>
-      <c r="Z18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:29">
-      <c r="A19" t="s">
-        <v>69</v>
-      </c>
-      <c r="B19" t="s">
-        <v>63</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -2313,25 +2528,31 @@
       <c r="U19">
         <v>0</v>
       </c>
-      <c r="W19" t="s">
-        <v>69</v>
-      </c>
-      <c r="X19" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y19">
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <v>0</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA19">
         <v>1E-3</v>
       </c>
-      <c r="Z19">
+      <c r="AB19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:29">
+    <row r="20" spans="1:31">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="B20" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -2390,66 +2611,381 @@
       <c r="U20">
         <v>1</v>
       </c>
-      <c r="W20" t="s">
-        <v>68</v>
-      </c>
-      <c r="X20" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y20">
+      <c r="V20">
+        <v>0</v>
+      </c>
+      <c r="W20">
+        <v>0</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA20">
         <v>1E-3</v>
       </c>
-      <c r="Z20">
+      <c r="AB20">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:29">
+    <row r="21" spans="1:31">
       <c r="A21" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B21" t="s">
-        <v>81</v>
-      </c>
-      <c r="W21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>-1</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <v>-1</v>
+      </c>
+      <c r="V21">
+        <v>1</v>
+      </c>
+      <c r="W21">
+        <v>0</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA21">
+        <v>1E-3</v>
+      </c>
+      <c r="AB21">
+        <v>1</v>
+      </c>
+      <c r="AC21" s="3"/>
+    </row>
+    <row r="22" spans="1:31">
+      <c r="A22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" t="s">
         <v>78</v>
       </c>
-      <c r="AA21" s="3"/>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>0</v>
+      </c>
+      <c r="T22">
+        <v>0</v>
+      </c>
+      <c r="U22">
+        <v>1</v>
+      </c>
+      <c r="V22">
+        <v>-1</v>
+      </c>
+      <c r="W22">
+        <v>0</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA22">
+        <v>0.01</v>
+      </c>
+      <c r="AB22">
+        <v>1</v>
+      </c>
+      <c r="AC22" s="3"/>
     </row>
-    <row r="22" spans="1:29">
-      <c r="A22" t="s">
-        <v>79</v>
-      </c>
-      <c r="B22" t="s">
+    <row r="23" spans="1:31">
+      <c r="A23" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" t="s">
         <v>82</v>
       </c>
-      <c r="AA22" s="3"/>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>-1</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <v>0</v>
+      </c>
+      <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="V23">
+        <v>0</v>
+      </c>
+      <c r="W23">
+        <v>0</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA23">
+        <v>1E-3</v>
+      </c>
+      <c r="AB23">
+        <v>1</v>
+      </c>
+      <c r="AC23" s="3"/>
     </row>
-    <row r="23" spans="1:29">
-      <c r="AA23" s="3"/>
+    <row r="24" spans="1:31">
+      <c r="A24" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+      <c r="R24">
+        <v>1</v>
+      </c>
+      <c r="S24">
+        <v>0</v>
+      </c>
+      <c r="T24">
+        <v>0</v>
+      </c>
+      <c r="U24">
+        <v>0</v>
+      </c>
+      <c r="V24">
+        <v>0</v>
+      </c>
+      <c r="W24">
+        <v>-1</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA24">
+        <v>1E-3</v>
+      </c>
+      <c r="AB24">
+        <v>1</v>
+      </c>
+      <c r="AC24" s="3"/>
     </row>
-    <row r="24" spans="1:29">
-      <c r="AA24" s="3"/>
+    <row r="25" spans="1:31">
+      <c r="AC25" s="3"/>
     </row>
-    <row r="25" spans="1:29">
-      <c r="AA25" s="3"/>
+    <row r="26" spans="1:31">
+      <c r="AC26" s="3"/>
     </row>
-    <row r="26" spans="1:29">
-      <c r="AA26" s="3"/>
+    <row r="27" spans="1:31" s="2" customFormat="1">
+      <c r="AC27" s="4"/>
     </row>
-    <row r="27" spans="1:29" s="2" customFormat="1">
-      <c r="AA27" s="4"/>
+    <row r="28" spans="1:31">
+      <c r="B28" s="1"/>
+      <c r="AC28" s="5"/>
     </row>
-    <row r="28" spans="1:29">
-      <c r="B28" s="1"/>
-      <c r="AA28" s="5"/>
+    <row r="29" spans="1:31" s="2" customFormat="1">
+      <c r="AC29" s="5"/>
     </row>
-    <row r="29" spans="1:29" s="2" customFormat="1">
-      <c r="AA29" s="5"/>
-    </row>
-    <row r="30" spans="1:29">
-      <c r="Z30" s="1"/>
-      <c r="AA30" s="5"/>
-      <c r="AC30" s="1"/>
+    <row r="30" spans="1:31">
+      <c r="AB30" s="1"/>
+      <c r="AC30" s="5"/>
+      <c r="AE30" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Im adding all my files originally
</commit_message>
<xml_diff>
--- a/lab_report_2_time_series/modeling/Chris_versions/model_values_simple_11092014.xlsx
+++ b/lab_report_2_time_series/modeling/Chris_versions/model_values_simple_11092014.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5500" yWindow="0" windowWidth="25600" windowHeight="14400"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14420"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="98">
   <si>
     <t>x1</t>
   </si>
@@ -291,6 +291,30 @@
   </si>
   <si>
     <t>x21</t>
+  </si>
+  <si>
+    <t>Inhibitor</t>
+  </si>
+  <si>
+    <t>x22</t>
+  </si>
+  <si>
+    <t>Inhibition of target</t>
+  </si>
+  <si>
+    <t>k23</t>
+  </si>
+  <si>
+    <t>Increasing Inhib concentration</t>
+  </si>
+  <si>
+    <t>k24</t>
+  </si>
+  <si>
+    <t>MEK deactivation</t>
+  </si>
+  <si>
+    <t>SOS activation by actTGFa_EGFR</t>
   </si>
 </sst>
 </file>
@@ -346,8 +370,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="165">
+  <cellStyleXfs count="177">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -521,7 +557,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="165">
+  <cellStyles count="177">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -604,6 +640,12 @@
     <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -686,6 +728,12 @@
     <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -985,10 +1033,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE30"/>
+  <dimension ref="A1:AF30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -996,11 +1044,11 @@
     <col min="1" max="1" width="25.5" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="12.83203125" customWidth="1"/>
     <col min="22" max="22" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.1640625" customWidth="1"/>
-    <col min="25" max="25" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="12.1640625" customWidth="1"/>
+    <col min="26" max="26" width="25.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:29">
       <c r="C1" t="s">
         <v>72</v>
       </c>
@@ -1064,8 +1112,11 @@
       <c r="W1" t="s">
         <v>61</v>
       </c>
+      <c r="X1" t="s">
+        <v>90</v>
+      </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:29">
       <c r="C2" t="s">
         <v>0</v>
       </c>
@@ -1129,14 +1180,17 @@
       <c r="W2" t="s">
         <v>89</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="X2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB2" t="s">
         <v>17</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:29">
       <c r="A3" t="s">
         <v>71</v>
       </c>
@@ -1206,20 +1260,23 @@
       <c r="W3">
         <v>0</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Z3" t="s">
         <v>71</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>10</v>
       </c>
-      <c r="AA3">
+      <c r="AB3">
         <v>1E-3</v>
       </c>
-      <c r="AB3">
+      <c r="AC3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:28">
+    <row r="4" spans="1:29">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -1227,7 +1284,7 @@
         <v>11</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1275,7 +1332,7 @@
         <v>0</v>
       </c>
       <c r="S4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T4">
         <v>0</v>
@@ -1289,20 +1346,23 @@
       <c r="W4">
         <v>0</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Z4" t="s">
         <v>73</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AA4" t="s">
         <v>11</v>
       </c>
-      <c r="AA4">
+      <c r="AB4">
         <v>0.01</v>
       </c>
-      <c r="AB4">
+      <c r="AC4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:28">
+    <row r="5" spans="1:29">
       <c r="A5" t="s">
         <v>81</v>
       </c>
@@ -1372,20 +1432,23 @@
       <c r="W5">
         <v>0</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Z5" t="s">
         <v>81</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AA5" t="s">
         <v>12</v>
       </c>
-      <c r="AA5">
+      <c r="AB5">
         <v>1E-3</v>
       </c>
-      <c r="AB5">
+      <c r="AC5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:28">
+    <row r="6" spans="1:29">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -1455,20 +1518,23 @@
       <c r="W6">
         <v>0</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Z6" t="s">
         <v>33</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AA6" t="s">
         <v>13</v>
       </c>
-      <c r="AA6">
-        <v>0.01</v>
-      </c>
       <c r="AB6">
+        <v>0.1</v>
+      </c>
+      <c r="AC6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:28">
+    <row r="7" spans="1:29">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -1538,20 +1604,23 @@
       <c r="W7">
         <v>0</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Z7" t="s">
         <v>44</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="AA7" t="s">
         <v>14</v>
       </c>
-      <c r="AA7">
+      <c r="AB7">
         <v>1E-3</v>
       </c>
-      <c r="AB7">
+      <c r="AC7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:28">
+    <row r="8" spans="1:29">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -1621,20 +1690,23 @@
       <c r="W8">
         <v>0</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Z8" t="s">
         <v>34</v>
       </c>
-      <c r="Z8" t="s">
+      <c r="AA8" t="s">
         <v>15</v>
       </c>
-      <c r="AA8">
-        <v>0.01</v>
-      </c>
       <c r="AB8">
+        <v>0.1</v>
+      </c>
+      <c r="AC8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:28">
+    <row r="9" spans="1:29">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -1704,20 +1776,23 @@
       <c r="W9">
         <v>0</v>
       </c>
-      <c r="Y9" t="s">
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Z9" t="s">
         <v>45</v>
       </c>
-      <c r="Z9" t="s">
+      <c r="AA9" t="s">
         <v>38</v>
       </c>
-      <c r="AA9">
+      <c r="AB9">
         <v>1E-3</v>
       </c>
-      <c r="AB9">
+      <c r="AC9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:28">
+    <row r="10" spans="1:29">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -1787,20 +1862,23 @@
       <c r="W10">
         <v>0</v>
       </c>
-      <c r="Y10" t="s">
+      <c r="X10">
+        <v>0</v>
+      </c>
+      <c r="Z10" t="s">
         <v>35</v>
       </c>
-      <c r="Z10" t="s">
+      <c r="AA10" t="s">
         <v>39</v>
       </c>
-      <c r="AA10">
-        <v>0.01</v>
-      </c>
       <c r="AB10">
+        <v>0.1</v>
+      </c>
+      <c r="AC10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:28">
+    <row r="11" spans="1:29">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -1870,20 +1948,23 @@
       <c r="W11">
         <v>0</v>
       </c>
-      <c r="Y11" t="s">
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Z11" t="s">
         <v>46</v>
       </c>
-      <c r="Z11" t="s">
+      <c r="AA11" t="s">
         <v>40</v>
       </c>
-      <c r="AA11">
+      <c r="AB11">
         <v>1E-3</v>
       </c>
-      <c r="AB11">
+      <c r="AC11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:28">
+    <row r="12" spans="1:29">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -1953,20 +2034,23 @@
       <c r="W12">
         <v>0</v>
       </c>
-      <c r="Y12" t="s">
-        <v>36</v>
+      <c r="X12">
+        <v>0</v>
       </c>
       <c r="Z12" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA12" t="s">
         <v>41</v>
       </c>
-      <c r="AA12">
-        <v>0.01</v>
-      </c>
       <c r="AB12">
+        <v>0.1</v>
+      </c>
+      <c r="AC12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:28">
+    <row r="13" spans="1:29">
       <c r="A13" t="s">
         <v>47</v>
       </c>
@@ -2036,20 +2120,23 @@
       <c r="W13">
         <v>0</v>
       </c>
-      <c r="Y13" t="s">
+      <c r="X13">
+        <v>0</v>
+      </c>
+      <c r="Z13" t="s">
         <v>47</v>
       </c>
-      <c r="Z13" t="s">
+      <c r="AA13" t="s">
         <v>42</v>
       </c>
-      <c r="AA13">
+      <c r="AB13">
         <v>1E-3</v>
       </c>
-      <c r="AB13">
+      <c r="AC13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:28">
+    <row r="14" spans="1:29">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -2119,20 +2206,23 @@
       <c r="W14">
         <v>0</v>
       </c>
-      <c r="Y14" t="s">
+      <c r="X14">
+        <v>0</v>
+      </c>
+      <c r="Z14" t="s">
         <v>37</v>
       </c>
-      <c r="Z14" t="s">
+      <c r="AA14" t="s">
         <v>43</v>
       </c>
-      <c r="AA14">
-        <v>0.01</v>
-      </c>
       <c r="AB14">
+        <v>0.1</v>
+      </c>
+      <c r="AC14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:28">
+    <row r="15" spans="1:29">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -2202,20 +2292,23 @@
       <c r="W15">
         <v>0</v>
       </c>
-      <c r="Y15" t="s">
+      <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="Z15" t="s">
         <v>48</v>
       </c>
-      <c r="Z15" t="s">
+      <c r="AA15" t="s">
         <v>50</v>
       </c>
-      <c r="AA15">
-        <v>0.01</v>
-      </c>
       <c r="AB15">
+        <v>1E-4</v>
+      </c>
+      <c r="AC15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:28">
+    <row r="16" spans="1:29">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -2285,20 +2378,23 @@
       <c r="W16">
         <v>0</v>
       </c>
-      <c r="Y16" t="s">
+      <c r="X16">
+        <v>0</v>
+      </c>
+      <c r="Z16" t="s">
         <v>55</v>
       </c>
-      <c r="Z16" t="s">
+      <c r="AA16" t="s">
         <v>51</v>
       </c>
-      <c r="AA16">
+      <c r="AB16">
         <v>1E-3</v>
       </c>
-      <c r="AB16">
+      <c r="AC16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:31">
+    <row r="17" spans="1:32">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -2368,20 +2464,23 @@
       <c r="W17">
         <v>0</v>
       </c>
-      <c r="Y17" t="s">
+      <c r="X17">
+        <v>0</v>
+      </c>
+      <c r="Z17" t="s">
         <v>49</v>
       </c>
-      <c r="Z17" t="s">
+      <c r="AA17" t="s">
         <v>56</v>
       </c>
-      <c r="AA17">
-        <v>0.01</v>
-      </c>
       <c r="AB17">
+        <v>1E-4</v>
+      </c>
+      <c r="AC17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:31">
+    <row r="18" spans="1:32">
       <c r="A18" t="s">
         <v>54</v>
       </c>
@@ -2451,20 +2550,23 @@
       <c r="W18">
         <v>0</v>
       </c>
-      <c r="Y18" t="s">
+      <c r="X18">
+        <v>0</v>
+      </c>
+      <c r="Z18" t="s">
         <v>54</v>
       </c>
-      <c r="Z18" t="s">
+      <c r="AA18" t="s">
         <v>57</v>
       </c>
-      <c r="AA18">
+      <c r="AB18">
         <v>1E-3</v>
       </c>
-      <c r="AB18">
+      <c r="AC18">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:31">
+    <row r="19" spans="1:32">
       <c r="A19" t="s">
         <v>84</v>
       </c>
@@ -2534,20 +2636,23 @@
       <c r="W19">
         <v>0</v>
       </c>
-      <c r="Y19" t="s">
+      <c r="X19">
+        <v>0</v>
+      </c>
+      <c r="Z19" t="s">
         <v>66</v>
       </c>
-      <c r="Z19" t="s">
+      <c r="AA19" t="s">
         <v>60</v>
       </c>
-      <c r="AA19">
+      <c r="AB19">
         <v>1E-3</v>
       </c>
-      <c r="AB19">
+      <c r="AC19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:31">
+    <row r="20" spans="1:32">
       <c r="A20" t="s">
         <v>85</v>
       </c>
@@ -2617,20 +2722,23 @@
       <c r="W20">
         <v>0</v>
       </c>
-      <c r="Y20" t="s">
+      <c r="X20">
+        <v>0</v>
+      </c>
+      <c r="Z20" t="s">
         <v>65</v>
       </c>
-      <c r="Z20" t="s">
+      <c r="AA20" t="s">
         <v>67</v>
       </c>
-      <c r="AA20">
+      <c r="AB20">
         <v>1E-3</v>
       </c>
-      <c r="AB20">
+      <c r="AC20">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:31">
+    <row r="21" spans="1:32">
       <c r="A21" t="s">
         <v>76</v>
       </c>
@@ -2700,21 +2808,24 @@
       <c r="W21">
         <v>0</v>
       </c>
-      <c r="Y21" t="s">
+      <c r="X21">
+        <v>0</v>
+      </c>
+      <c r="Z21" t="s">
         <v>76</v>
       </c>
-      <c r="Z21" t="s">
+      <c r="AA21" t="s">
         <v>77</v>
       </c>
-      <c r="AA21">
+      <c r="AB21">
         <v>1E-3</v>
       </c>
-      <c r="AB21">
-        <v>1</v>
-      </c>
-      <c r="AC21" s="3"/>
+      <c r="AC21">
+        <v>1</v>
+      </c>
+      <c r="AD21" s="3"/>
     </row>
-    <row r="22" spans="1:31">
+    <row r="22" spans="1:32">
       <c r="A22" t="s">
         <v>75</v>
       </c>
@@ -2773,10 +2884,10 @@
         <v>0</v>
       </c>
       <c r="T22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V22">
         <v>-1</v>
@@ -2784,21 +2895,24 @@
       <c r="W22">
         <v>0</v>
       </c>
-      <c r="Y22" t="s">
+      <c r="X22">
+        <v>0</v>
+      </c>
+      <c r="Z22" t="s">
         <v>75</v>
       </c>
-      <c r="Z22" t="s">
+      <c r="AA22" t="s">
         <v>78</v>
       </c>
-      <c r="AA22">
+      <c r="AB22">
         <v>0.01</v>
       </c>
-      <c r="AB22">
-        <v>1</v>
-      </c>
-      <c r="AC22" s="3"/>
+      <c r="AC22">
+        <v>1</v>
+      </c>
+      <c r="AD22" s="3"/>
     </row>
-    <row r="23" spans="1:31">
+    <row r="23" spans="1:32">
       <c r="A23" t="s">
         <v>83</v>
       </c>
@@ -2868,21 +2982,24 @@
       <c r="W23">
         <v>0</v>
       </c>
-      <c r="Y23" t="s">
-        <v>83</v>
+      <c r="X23">
+        <v>0</v>
       </c>
       <c r="Z23" t="s">
+        <v>97</v>
+      </c>
+      <c r="AA23" t="s">
         <v>82</v>
       </c>
-      <c r="AA23">
+      <c r="AB23">
         <v>1E-3</v>
       </c>
-      <c r="AB23">
-        <v>1</v>
-      </c>
-      <c r="AC23" s="3"/>
+      <c r="AC23">
+        <v>1</v>
+      </c>
+      <c r="AD23" s="3"/>
     </row>
-    <row r="24" spans="1:31">
+    <row r="24" spans="1:32">
       <c r="A24" t="s">
         <v>87</v>
       </c>
@@ -2952,40 +3069,211 @@
       <c r="W24">
         <v>-1</v>
       </c>
-      <c r="Y24" t="s">
+      <c r="X24">
+        <v>0</v>
+      </c>
+      <c r="Z24" t="s">
         <v>87</v>
       </c>
-      <c r="Z24" t="s">
+      <c r="AA24" t="s">
         <v>88</v>
       </c>
-      <c r="AA24">
+      <c r="AB24">
         <v>1E-3</v>
       </c>
-      <c r="AB24">
-        <v>1</v>
-      </c>
-      <c r="AC24" s="3"/>
+      <c r="AC24">
+        <v>1</v>
+      </c>
+      <c r="AD24" s="3"/>
     </row>
-    <row r="25" spans="1:31">
-      <c r="AC25" s="3"/>
+    <row r="25" spans="1:32">
+      <c r="A25" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>-1</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+      <c r="R25">
+        <v>0</v>
+      </c>
+      <c r="S25">
+        <v>0</v>
+      </c>
+      <c r="T25">
+        <v>0</v>
+      </c>
+      <c r="U25">
+        <v>0</v>
+      </c>
+      <c r="V25">
+        <v>0</v>
+      </c>
+      <c r="W25">
+        <v>0</v>
+      </c>
+      <c r="X25">
+        <v>-1</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB25">
+        <v>0.01</v>
+      </c>
+      <c r="AC25">
+        <v>1</v>
+      </c>
+      <c r="AD25" s="3"/>
     </row>
-    <row r="26" spans="1:31">
-      <c r="AC26" s="3"/>
+    <row r="26" spans="1:32">
+      <c r="A26" t="s">
+        <v>94</v>
+      </c>
+      <c r="B26" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <v>0</v>
+      </c>
+      <c r="S26">
+        <v>0</v>
+      </c>
+      <c r="T26">
+        <v>0</v>
+      </c>
+      <c r="U26">
+        <v>0</v>
+      </c>
+      <c r="V26">
+        <v>0</v>
+      </c>
+      <c r="W26">
+        <v>0</v>
+      </c>
+      <c r="X26">
+        <v>1</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>95</v>
+      </c>
+      <c r="AB26">
+        <v>0.5</v>
+      </c>
+      <c r="AC26">
+        <v>0</v>
+      </c>
+      <c r="AD26" s="3"/>
     </row>
-    <row r="27" spans="1:31" s="2" customFormat="1">
-      <c r="AC27" s="4"/>
+    <row r="27" spans="1:32" s="2" customFormat="1">
+      <c r="AD27" s="4"/>
     </row>
-    <row r="28" spans="1:31">
+    <row r="28" spans="1:32">
       <c r="B28" s="1"/>
-      <c r="AC28" s="5"/>
+      <c r="AD28" s="5"/>
     </row>
-    <row r="29" spans="1:31" s="2" customFormat="1">
-      <c r="AC29" s="5"/>
+    <row r="29" spans="1:32" s="2" customFormat="1">
+      <c r="AD29" s="5"/>
     </row>
-    <row r="30" spans="1:31">
-      <c r="AB30" s="1"/>
-      <c r="AC30" s="5"/>
-      <c r="AE30" s="1"/>
+    <row r="30" spans="1:32">
+      <c r="AC30" s="1"/>
+      <c r="AD30" s="5"/>
+      <c r="AF30" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>